<commit_message>
first nes connection test. rom /ce seems not coming... must investigate.
</commit_message>
<xml_diff>
--- a/doc/universal-board-test.xlsx
+++ b/doc/universal-board-test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="21555" windowHeight="12120" activeTab="4"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="21555" windowHeight="12120" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="circuit-emu" sheetId="1" r:id="rId1"/>
@@ -12,6 +12,7 @@
     <sheet name="logic-analyzer-result" sheetId="2" r:id="rId3"/>
     <sheet name="universal-board" sheetId="5" r:id="rId4"/>
     <sheet name="board-inter-connect" sheetId="3" r:id="rId5"/>
+    <sheet name="nes-debug" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
@@ -47488,6 +47489,244 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1027" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="18154650" cy="2886075"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="角丸四角形吹き出し 3"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6438900" y="2971800"/>
+          <a:ext cx="1514475" cy="942975"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRoundRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -29009"/>
+            <a:gd name="adj2" fmla="val -94066"/>
+            <a:gd name="adj3" fmla="val 16667"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>push stack</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="角丸四角形吹き出し 4"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9229725" y="2809875"/>
+          <a:ext cx="1514475" cy="942975"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRoundRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -29009"/>
+            <a:gd name="adj2" fmla="val -94066"/>
+            <a:gd name="adj3" fmla="val 16667"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" b="1"/>
+            <a:t>fetch reset vector</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" b="1"/>
+            <a:t>rom /ce</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" b="1" baseline="0"/>
+            <a:t> doesn't set??</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" b="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="円/楕円 5"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8582025" y="1638300"/>
+          <a:ext cx="2905125" cy="504825"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent5">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office テーマ">
   <a:themeElements>
@@ -53840,7 +54079,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="G6:AS68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AQ41" sqref="AQ41"/>
     </sheetView>
   </sheetViews>
@@ -54666,4 +54905,20 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q21" sqref="Q21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetData/>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>